<commit_message>
second commint to Amazon
</commit_message>
<xml_diff>
--- a/Amazon_Cucumber/src/test/resources/DataProvider/Addaddress_Amazon.xlsx
+++ b/Amazon_Cucumber/src/test/resources/DataProvider/Addaddress_Amazon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Selenium\AdactinHotelBooking\src\test\resources\DataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkingDirectory\Amazon_Cucumber\src\test\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF3AC134-7221-48BF-AE8D-FF5940E2A02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE99908-A212-4C7F-8A73-B8EA51BF5C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="10433" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AmazonAddress" sheetId="1" r:id="rId1"/>
@@ -42,25 +42,25 @@
     <t>Mickro</t>
   </si>
   <si>
-    <t>LA</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
     <t>Phone number</t>
   </si>
   <si>
+    <t>ZIP Code</t>
+  </si>
+  <si>
+    <t>50048185479</t>
+  </si>
+  <si>
     <t>6666 E WASHINGTON BLVD</t>
   </si>
   <si>
-    <t>ZIP Code</t>
+    <t>COMMERCE</t>
   </si>
   <si>
     <t>90040</t>
-  </si>
-  <si>
-    <t>50048185479</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -447,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -468,19 +468,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="4"/>
     </row>

</xml_diff>